<commit_message>
SLL64 errors fixed (not tested)
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-0799-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-0799-350-1201.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\Ensc_350\Assignments-350\1201\Labwork\FP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC6787F-6BB0-486B-95D5-E5DACEAF45A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA02D22E-AA23-4E9E-9C83-9C0AFF24A4C8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log - Part 1" sheetId="5" r:id="rId1"/>
     <sheet name="Activity Log - Part 2" sheetId="4" r:id="rId2"/>
     <sheet name="Activity Log - Part 3" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -122,6 +122,27 @@
   </si>
   <si>
     <t>Gxx</t>
+  </si>
+  <si>
+    <t>Ruelt Yean (Ryan), Kiew</t>
+  </si>
+  <si>
+    <t>G47</t>
+  </si>
+  <si>
+    <t>Read through Part 2 pdf</t>
+  </si>
+  <si>
+    <t>Reviewed Barrel Shifter design implementation</t>
+  </si>
+  <si>
+    <t>First implementation  of Barrel Shifter</t>
+  </si>
+  <si>
+    <t>Second implementation of Barrel Shifter; attempting to use same MUX entity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Third implementaiton of Barrel Shifter; error fixing, split MUX into three entities </t>
   </si>
 </sst>
 </file>
@@ -920,7 +941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090E6E40-83BD-4CBB-97D3-102021CD8368}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -1010,7 +1031,7 @@
       <c r="F6" s="32"/>
       <c r="G6" s="16"/>
       <c r="H6" s="12">
-        <f t="shared" ref="H6" si="0">(E6-D6)*24</f>
+        <f>(E6-D6)*24</f>
         <v>0</v>
       </c>
       <c r="I6" s="10"/>
@@ -1037,7 +1058,7 @@
       <c r="F8" s="34"/>
       <c r="G8" s="17"/>
       <c r="H8" s="27">
-        <f t="shared" ref="H8:H71" si="1">(E8-D8)*24</f>
+        <f t="shared" ref="H8:H71" si="0">(E8-D8)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -1050,7 +1071,7 @@
       <c r="F9" s="34"/>
       <c r="G9" s="17"/>
       <c r="H9" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1063,7 +1084,7 @@
       <c r="F10" s="34"/>
       <c r="G10" s="17"/>
       <c r="H10" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1076,7 +1097,7 @@
       <c r="F11" s="34"/>
       <c r="G11" s="17"/>
       <c r="H11" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1089,7 +1110,7 @@
       <c r="F12" s="34"/>
       <c r="G12" s="17"/>
       <c r="H12" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1102,7 +1123,7 @@
       <c r="F13" s="34"/>
       <c r="G13" s="17"/>
       <c r="H13" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1115,7 +1136,7 @@
       <c r="F14" s="34"/>
       <c r="G14" s="17"/>
       <c r="H14" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1128,7 +1149,7 @@
       <c r="F15" s="34"/>
       <c r="G15" s="17"/>
       <c r="H15" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1141,7 +1162,7 @@
       <c r="F16" s="34"/>
       <c r="G16" s="17"/>
       <c r="H16" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1154,7 +1175,7 @@
       <c r="F17" s="34"/>
       <c r="G17" s="17"/>
       <c r="H17" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1167,7 +1188,7 @@
       <c r="F18" s="34"/>
       <c r="G18" s="17"/>
       <c r="H18" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1180,7 +1201,7 @@
       <c r="F19" s="34"/>
       <c r="G19" s="17"/>
       <c r="H19" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1193,7 +1214,7 @@
       <c r="F20" s="34"/>
       <c r="G20" s="17"/>
       <c r="H20" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1206,7 +1227,7 @@
       <c r="F21" s="34"/>
       <c r="G21" s="17"/>
       <c r="H21" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1219,7 +1240,7 @@
       <c r="F22" s="34"/>
       <c r="G22" s="17"/>
       <c r="H22" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1232,7 +1253,7 @@
       <c r="F23" s="34"/>
       <c r="G23" s="17"/>
       <c r="H23" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1245,7 +1266,7 @@
       <c r="F24" s="34"/>
       <c r="G24" s="17"/>
       <c r="H24" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1258,7 +1279,7 @@
       <c r="F25" s="34"/>
       <c r="G25" s="17"/>
       <c r="H25" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1271,7 +1292,7 @@
       <c r="F26" s="34"/>
       <c r="G26" s="17"/>
       <c r="H26" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1284,7 +1305,7 @@
       <c r="F27" s="34"/>
       <c r="G27" s="17"/>
       <c r="H27" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1297,7 +1318,7 @@
       <c r="F28" s="34"/>
       <c r="G28" s="17"/>
       <c r="H28" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1310,7 +1331,7 @@
       <c r="F29" s="34"/>
       <c r="G29" s="17"/>
       <c r="H29" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1323,7 +1344,7 @@
       <c r="F30" s="34"/>
       <c r="G30" s="17"/>
       <c r="H30" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1336,7 +1357,7 @@
       <c r="F31" s="34"/>
       <c r="G31" s="17"/>
       <c r="H31" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1349,7 +1370,7 @@
       <c r="F32" s="34"/>
       <c r="G32" s="17"/>
       <c r="H32" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1362,7 +1383,7 @@
       <c r="F33" s="34"/>
       <c r="G33" s="17"/>
       <c r="H33" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1375,7 +1396,7 @@
       <c r="F34" s="34"/>
       <c r="G34" s="17"/>
       <c r="H34" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1388,7 +1409,7 @@
       <c r="F35" s="34"/>
       <c r="G35" s="17"/>
       <c r="H35" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1401,7 +1422,7 @@
       <c r="F36" s="34"/>
       <c r="G36" s="17"/>
       <c r="H36" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1414,7 +1435,7 @@
       <c r="F37" s="34"/>
       <c r="G37" s="17"/>
       <c r="H37" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1427,7 +1448,7 @@
       <c r="F38" s="34"/>
       <c r="G38" s="17"/>
       <c r="H38" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1440,7 +1461,7 @@
       <c r="F39" s="34"/>
       <c r="G39" s="17"/>
       <c r="H39" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1453,7 +1474,7 @@
       <c r="F40" s="34"/>
       <c r="G40" s="17"/>
       <c r="H40" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1466,7 +1487,7 @@
       <c r="F41" s="34"/>
       <c r="G41" s="17"/>
       <c r="H41" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1479,7 +1500,7 @@
       <c r="F42" s="34"/>
       <c r="G42" s="17"/>
       <c r="H42" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1492,7 +1513,7 @@
       <c r="F43" s="34"/>
       <c r="G43" s="17"/>
       <c r="H43" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1505,7 +1526,7 @@
       <c r="F44" s="34"/>
       <c r="G44" s="17"/>
       <c r="H44" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1518,7 +1539,7 @@
       <c r="F45" s="34"/>
       <c r="G45" s="17"/>
       <c r="H45" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1531,7 +1552,7 @@
       <c r="F46" s="34"/>
       <c r="G46" s="17"/>
       <c r="H46" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1544,7 +1565,7 @@
       <c r="F47" s="34"/>
       <c r="G47" s="17"/>
       <c r="H47" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1557,7 +1578,7 @@
       <c r="F48" s="34"/>
       <c r="G48" s="17"/>
       <c r="H48" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1570,7 +1591,7 @@
       <c r="F49" s="34"/>
       <c r="G49" s="17"/>
       <c r="H49" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1583,7 +1604,7 @@
       <c r="F50" s="34"/>
       <c r="G50" s="17"/>
       <c r="H50" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1596,7 +1617,7 @@
       <c r="F51" s="34"/>
       <c r="G51" s="17"/>
       <c r="H51" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1609,7 +1630,7 @@
       <c r="F52" s="34"/>
       <c r="G52" s="17"/>
       <c r="H52" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1622,7 +1643,7 @@
       <c r="F53" s="34"/>
       <c r="G53" s="17"/>
       <c r="H53" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1635,7 +1656,7 @@
       <c r="F54" s="34"/>
       <c r="G54" s="17"/>
       <c r="H54" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1648,7 +1669,7 @@
       <c r="F55" s="34"/>
       <c r="G55" s="17"/>
       <c r="H55" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1661,7 +1682,7 @@
       <c r="F56" s="34"/>
       <c r="G56" s="17"/>
       <c r="H56" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1674,7 +1695,7 @@
       <c r="F57" s="34"/>
       <c r="G57" s="17"/>
       <c r="H57" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1687,7 +1708,7 @@
       <c r="F58" s="34"/>
       <c r="G58" s="17"/>
       <c r="H58" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1700,7 +1721,7 @@
       <c r="F59" s="34"/>
       <c r="G59" s="17"/>
       <c r="H59" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1713,7 +1734,7 @@
       <c r="F60" s="34"/>
       <c r="G60" s="17"/>
       <c r="H60" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1726,7 +1747,7 @@
       <c r="F61" s="34"/>
       <c r="G61" s="17"/>
       <c r="H61" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1739,7 +1760,7 @@
       <c r="F62" s="34"/>
       <c r="G62" s="17"/>
       <c r="H62" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1752,7 +1773,7 @@
       <c r="F63" s="34"/>
       <c r="G63" s="17"/>
       <c r="H63" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1765,7 +1786,7 @@
       <c r="F64" s="34"/>
       <c r="G64" s="17"/>
       <c r="H64" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1778,7 +1799,7 @@
       <c r="F65" s="34"/>
       <c r="G65" s="17"/>
       <c r="H65" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1791,7 +1812,7 @@
       <c r="F66" s="34"/>
       <c r="G66" s="17"/>
       <c r="H66" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1804,7 +1825,7 @@
       <c r="F67" s="34"/>
       <c r="G67" s="17"/>
       <c r="H67" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1817,7 +1838,7 @@
       <c r="F68" s="34"/>
       <c r="G68" s="17"/>
       <c r="H68" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1830,7 +1851,7 @@
       <c r="F69" s="34"/>
       <c r="G69" s="17"/>
       <c r="H69" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1843,7 +1864,7 @@
       <c r="F70" s="34"/>
       <c r="G70" s="17"/>
       <c r="H70" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1856,7 +1877,7 @@
       <c r="F71" s="34"/>
       <c r="G71" s="17"/>
       <c r="H71" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1869,7 +1890,7 @@
       <c r="F72" s="34"/>
       <c r="G72" s="17"/>
       <c r="H72" s="27">
-        <f t="shared" ref="H72:H78" si="2">(E72-D72)*24</f>
+        <f t="shared" ref="H72:H78" si="1">(E72-D72)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -1882,7 +1903,7 @@
       <c r="F73" s="34"/>
       <c r="G73" s="17"/>
       <c r="H73" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1895,7 +1916,7 @@
       <c r="F74" s="34"/>
       <c r="G74" s="17"/>
       <c r="H74" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1908,7 +1929,7 @@
       <c r="F75" s="34"/>
       <c r="G75" s="17"/>
       <c r="H75" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1921,7 +1942,7 @@
       <c r="F76" s="34"/>
       <c r="G76" s="17"/>
       <c r="H76" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1934,7 +1955,7 @@
       <c r="F77" s="34"/>
       <c r="G77" s="17"/>
       <c r="H77" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1947,7 +1968,7 @@
       <c r="F78" s="36"/>
       <c r="G78" s="18"/>
       <c r="H78" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2684,7 +2705,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A6" sqref="A6:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2773,7 +2794,7 @@
       <c r="F6" s="32"/>
       <c r="G6" s="16"/>
       <c r="H6" s="12">
-        <f t="shared" ref="H6" si="0">(E6-D6)*24</f>
+        <f>(E6-D6)*24</f>
         <v>0</v>
       </c>
       <c r="I6" s="10"/>
@@ -2800,7 +2821,7 @@
       <c r="F8" s="34"/>
       <c r="G8" s="17"/>
       <c r="H8" s="27">
-        <f t="shared" ref="H8:H71" si="1">(E8-D8)*24</f>
+        <f>(E8-D8)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -2813,7 +2834,7 @@
       <c r="F9" s="34"/>
       <c r="G9" s="17"/>
       <c r="H9" s="27">
-        <f t="shared" si="1"/>
+        <f>(E9-D9)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -2826,7 +2847,7 @@
       <c r="F10" s="34"/>
       <c r="G10" s="17"/>
       <c r="H10" s="27">
-        <f t="shared" si="1"/>
+        <f>(E10-D10)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -2839,7 +2860,7 @@
       <c r="F11" s="34"/>
       <c r="G11" s="17"/>
       <c r="H11" s="27">
-        <f t="shared" si="1"/>
+        <f>(E11-D11)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -2852,7 +2873,7 @@
       <c r="F12" s="34"/>
       <c r="G12" s="17"/>
       <c r="H12" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H12:H71" si="0">(E12-D12)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -2865,7 +2886,7 @@
       <c r="F13" s="34"/>
       <c r="G13" s="17"/>
       <c r="H13" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2878,7 +2899,7 @@
       <c r="F14" s="34"/>
       <c r="G14" s="17"/>
       <c r="H14" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2891,7 +2912,7 @@
       <c r="F15" s="34"/>
       <c r="G15" s="17"/>
       <c r="H15" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2904,7 +2925,7 @@
       <c r="F16" s="34"/>
       <c r="G16" s="17"/>
       <c r="H16" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2917,7 +2938,7 @@
       <c r="F17" s="34"/>
       <c r="G17" s="17"/>
       <c r="H17" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2930,7 +2951,7 @@
       <c r="F18" s="34"/>
       <c r="G18" s="17"/>
       <c r="H18" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2943,7 +2964,7 @@
       <c r="F19" s="34"/>
       <c r="G19" s="17"/>
       <c r="H19" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2956,7 +2977,7 @@
       <c r="F20" s="34"/>
       <c r="G20" s="17"/>
       <c r="H20" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2969,7 +2990,7 @@
       <c r="F21" s="34"/>
       <c r="G21" s="17"/>
       <c r="H21" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2982,7 +3003,7 @@
       <c r="F22" s="34"/>
       <c r="G22" s="17"/>
       <c r="H22" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3008,7 +3029,7 @@
       <c r="F24" s="34"/>
       <c r="G24" s="17"/>
       <c r="H24" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3021,7 +3042,7 @@
       <c r="F25" s="34"/>
       <c r="G25" s="17"/>
       <c r="H25" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3034,7 +3055,7 @@
       <c r="F26" s="34"/>
       <c r="G26" s="17"/>
       <c r="H26" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3047,7 +3068,7 @@
       <c r="F27" s="34"/>
       <c r="G27" s="17"/>
       <c r="H27" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3060,7 +3081,7 @@
       <c r="F28" s="34"/>
       <c r="G28" s="17"/>
       <c r="H28" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3073,7 +3094,7 @@
       <c r="F29" s="34"/>
       <c r="G29" s="17"/>
       <c r="H29" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3086,7 +3107,7 @@
       <c r="F30" s="34"/>
       <c r="G30" s="17"/>
       <c r="H30" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3099,7 +3120,7 @@
       <c r="F31" s="34"/>
       <c r="G31" s="17"/>
       <c r="H31" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3112,7 +3133,7 @@
       <c r="F32" s="34"/>
       <c r="G32" s="17"/>
       <c r="H32" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3125,7 +3146,7 @@
       <c r="F33" s="34"/>
       <c r="G33" s="17"/>
       <c r="H33" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3138,7 +3159,7 @@
       <c r="F34" s="34"/>
       <c r="G34" s="17"/>
       <c r="H34" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3151,7 +3172,7 @@
       <c r="F35" s="34"/>
       <c r="G35" s="17"/>
       <c r="H35" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3164,7 +3185,7 @@
       <c r="F36" s="34"/>
       <c r="G36" s="17"/>
       <c r="H36" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3177,7 +3198,7 @@
       <c r="F37" s="34"/>
       <c r="G37" s="17"/>
       <c r="H37" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3190,7 +3211,7 @@
       <c r="F38" s="34"/>
       <c r="G38" s="17"/>
       <c r="H38" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3203,7 +3224,7 @@
       <c r="F39" s="34"/>
       <c r="G39" s="17"/>
       <c r="H39" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3216,7 +3237,7 @@
       <c r="F40" s="34"/>
       <c r="G40" s="17"/>
       <c r="H40" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3229,7 +3250,7 @@
       <c r="F41" s="34"/>
       <c r="G41" s="17"/>
       <c r="H41" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3242,7 +3263,7 @@
       <c r="F42" s="34"/>
       <c r="G42" s="17"/>
       <c r="H42" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3255,7 +3276,7 @@
       <c r="F43" s="34"/>
       <c r="G43" s="17"/>
       <c r="H43" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3268,7 +3289,7 @@
       <c r="F44" s="34"/>
       <c r="G44" s="17"/>
       <c r="H44" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3281,7 +3302,7 @@
       <c r="F45" s="34"/>
       <c r="G45" s="17"/>
       <c r="H45" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3294,7 +3315,7 @@
       <c r="F46" s="34"/>
       <c r="G46" s="17"/>
       <c r="H46" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3307,7 +3328,7 @@
       <c r="F47" s="34"/>
       <c r="G47" s="17"/>
       <c r="H47" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3320,7 +3341,7 @@
       <c r="F48" s="34"/>
       <c r="G48" s="17"/>
       <c r="H48" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3333,7 +3354,7 @@
       <c r="F49" s="34"/>
       <c r="G49" s="17"/>
       <c r="H49" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3346,7 +3367,7 @@
       <c r="F50" s="34"/>
       <c r="G50" s="17"/>
       <c r="H50" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3359,7 +3380,7 @@
       <c r="F51" s="34"/>
       <c r="G51" s="17"/>
       <c r="H51" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3372,7 +3393,7 @@
       <c r="F52" s="34"/>
       <c r="G52" s="17"/>
       <c r="H52" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3385,7 +3406,7 @@
       <c r="F53" s="34"/>
       <c r="G53" s="17"/>
       <c r="H53" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3398,7 +3419,7 @@
       <c r="F54" s="34"/>
       <c r="G54" s="17"/>
       <c r="H54" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3411,7 +3432,7 @@
       <c r="F55" s="34"/>
       <c r="G55" s="17"/>
       <c r="H55" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3424,7 +3445,7 @@
       <c r="F56" s="34"/>
       <c r="G56" s="17"/>
       <c r="H56" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3437,7 +3458,7 @@
       <c r="F57" s="34"/>
       <c r="G57" s="17"/>
       <c r="H57" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3450,7 +3471,7 @@
       <c r="F58" s="34"/>
       <c r="G58" s="17"/>
       <c r="H58" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3463,7 +3484,7 @@
       <c r="F59" s="34"/>
       <c r="G59" s="17"/>
       <c r="H59" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3476,7 +3497,7 @@
       <c r="F60" s="34"/>
       <c r="G60" s="17"/>
       <c r="H60" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3489,7 +3510,7 @@
       <c r="F61" s="34"/>
       <c r="G61" s="17"/>
       <c r="H61" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3502,7 +3523,7 @@
       <c r="F62" s="34"/>
       <c r="G62" s="17"/>
       <c r="H62" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3515,7 +3536,7 @@
       <c r="F63" s="34"/>
       <c r="G63" s="17"/>
       <c r="H63" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3528,7 +3549,7 @@
       <c r="F64" s="34"/>
       <c r="G64" s="17"/>
       <c r="H64" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3541,7 +3562,7 @@
       <c r="F65" s="34"/>
       <c r="G65" s="17"/>
       <c r="H65" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3554,7 +3575,7 @@
       <c r="F66" s="34"/>
       <c r="G66" s="17"/>
       <c r="H66" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3567,7 +3588,7 @@
       <c r="F67" s="34"/>
       <c r="G67" s="17"/>
       <c r="H67" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3580,7 +3601,7 @@
       <c r="F68" s="34"/>
       <c r="G68" s="17"/>
       <c r="H68" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3593,7 +3614,7 @@
       <c r="F69" s="34"/>
       <c r="G69" s="17"/>
       <c r="H69" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3606,7 +3627,7 @@
       <c r="F70" s="34"/>
       <c r="G70" s="17"/>
       <c r="H70" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3619,7 +3640,7 @@
       <c r="F71" s="34"/>
       <c r="G71" s="17"/>
       <c r="H71" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3632,7 +3653,7 @@
       <c r="F72" s="34"/>
       <c r="G72" s="17"/>
       <c r="H72" s="27">
-        <f t="shared" ref="H72:H78" si="2">(E72-D72)*24</f>
+        <f t="shared" ref="H72:H78" si="1">(E72-D72)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -3645,7 +3666,7 @@
       <c r="F73" s="34"/>
       <c r="G73" s="17"/>
       <c r="H73" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3658,7 +3679,7 @@
       <c r="F74" s="34"/>
       <c r="G74" s="17"/>
       <c r="H74" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3671,7 +3692,7 @@
       <c r="F75" s="34"/>
       <c r="G75" s="17"/>
       <c r="H75" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3684,7 +3705,7 @@
       <c r="F76" s="34"/>
       <c r="G76" s="17"/>
       <c r="H76" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3697,7 +3718,7 @@
       <c r="F77" s="34"/>
       <c r="G77" s="17"/>
       <c r="H77" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3710,7 +3731,7 @@
       <c r="F78" s="36"/>
       <c r="G78" s="18"/>
       <c r="H78" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4467,7 +4488,9 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="37" t="s">
+        <v>14</v>
+      </c>
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
       <c r="E1" s="38" t="s">
@@ -4480,7 +4503,9 @@
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="39"/>
+      <c r="B2" s="39">
+        <v>301290779</v>
+      </c>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
       <c r="E2" s="38"/>
@@ -4492,7 +4517,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
@@ -4529,94 +4554,146 @@
     </row>
     <row r="6" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
+      <c r="B6" s="13">
+        <v>779</v>
+      </c>
+      <c r="C6" s="19">
+        <v>43931</v>
+      </c>
+      <c r="D6" s="20">
+        <v>0.64513888888888882</v>
+      </c>
+      <c r="E6" s="21">
+        <v>0.65555555555555556</v>
+      </c>
       <c r="F6" s="32"/>
-      <c r="G6" s="16"/>
+      <c r="G6" s="16" t="s">
+        <v>16</v>
+      </c>
       <c r="H6" s="12">
-        <f t="shared" ref="H6" si="0">(E6-D6)*24</f>
-        <v>0</v>
+        <f>(E6-D6)*24</f>
+        <v>0.25000000000000178</v>
       </c>
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="23"/>
+      <c r="B7" s="14">
+        <v>779</v>
+      </c>
+      <c r="C7" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D7" s="20">
+        <v>0.65555555555555556</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0.66180555555555554</v>
+      </c>
       <c r="F7" s="34"/>
-      <c r="G7" s="17"/>
+      <c r="G7" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="H7" s="27">
         <f>(E7-D7)*24</f>
-        <v>0</v>
+        <v>0.14999999999999947</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="23"/>
+      <c r="C8" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D8" s="20">
+        <v>0.72638888888888886</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0.75138888888888899</v>
+      </c>
       <c r="F8" s="34"/>
-      <c r="G8" s="17"/>
+      <c r="G8" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="H8" s="27">
-        <f t="shared" ref="H8:H71" si="1">(E8-D8)*24</f>
-        <v>0</v>
+        <f>(E8-D8)*24</f>
+        <v>0.6000000000000032</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="33"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="23"/>
+      <c r="C9" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0.84097222222222223</v>
+      </c>
+      <c r="E9" s="23">
+        <v>0.94027777777777777</v>
+      </c>
       <c r="F9" s="34"/>
-      <c r="G9" s="17"/>
+      <c r="G9" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="H9" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>(E9-D9)*24</f>
+        <v>2.3833333333333329</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33"/>
       <c r="B10" s="14"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="23"/>
+      <c r="C10" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D10" s="20">
+        <v>0.58958333333333335</v>
+      </c>
+      <c r="E10" s="23">
+        <v>0.6069444444444444</v>
+      </c>
       <c r="F10" s="34"/>
       <c r="G10" s="17"/>
       <c r="H10" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>(E10-D10)*24</f>
+        <v>0.41666666666666519</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="33"/>
       <c r="B11" s="14"/>
       <c r="C11" s="22"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="23"/>
+      <c r="D11" s="20">
+        <v>0.83611111111111114</v>
+      </c>
+      <c r="E11" s="23">
+        <v>0.96111111111111114</v>
+      </c>
       <c r="F11" s="34"/>
       <c r="G11" s="17"/>
       <c r="H11" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>(E11-D11)*24</f>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33"/>
       <c r="B12" s="14"/>
       <c r="C12" s="22"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="23"/>
+      <c r="D12" s="20">
+        <v>0.4381944444444445</v>
+      </c>
+      <c r="E12" s="23">
+        <v>0.47291666666666665</v>
+      </c>
       <c r="F12" s="34"/>
-      <c r="G12" s="17"/>
+      <c r="G12" s="17" t="s">
+        <v>20</v>
+      </c>
       <c r="H12" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>(E12-D12)*24</f>
+        <v>0.83333333333333171</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4628,7 +4705,7 @@
       <c r="F13" s="34"/>
       <c r="G13" s="17"/>
       <c r="H13" s="27">
-        <f t="shared" si="1"/>
+        <f>(E13-D13)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4641,7 +4718,7 @@
       <c r="F14" s="34"/>
       <c r="G14" s="17"/>
       <c r="H14" s="27">
-        <f t="shared" si="1"/>
+        <f>(E14-D14)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4654,7 +4731,7 @@
       <c r="F15" s="34"/>
       <c r="G15" s="17"/>
       <c r="H15" s="27">
-        <f t="shared" si="1"/>
+        <f>(E15-D15)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4667,7 +4744,7 @@
       <c r="F16" s="34"/>
       <c r="G16" s="17"/>
       <c r="H16" s="27">
-        <f t="shared" si="1"/>
+        <f>(E16-D16)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4680,7 +4757,7 @@
       <c r="F17" s="34"/>
       <c r="G17" s="17"/>
       <c r="H17" s="27">
-        <f t="shared" si="1"/>
+        <f>(E17-D17)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4693,7 +4770,7 @@
       <c r="F18" s="34"/>
       <c r="G18" s="17"/>
       <c r="H18" s="27">
-        <f t="shared" si="1"/>
+        <f>(E18-D18)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4706,7 +4783,7 @@
       <c r="F19" s="34"/>
       <c r="G19" s="17"/>
       <c r="H19" s="27">
-        <f t="shared" si="1"/>
+        <f>(E19-D19)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4719,7 +4796,7 @@
       <c r="F20" s="34"/>
       <c r="G20" s="17"/>
       <c r="H20" s="27">
-        <f t="shared" si="1"/>
+        <f>(E20-D20)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4732,7 +4809,7 @@
       <c r="F21" s="34"/>
       <c r="G21" s="17"/>
       <c r="H21" s="27">
-        <f t="shared" si="1"/>
+        <f>(E21-D21)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4745,7 +4822,7 @@
       <c r="F22" s="34"/>
       <c r="G22" s="17"/>
       <c r="H22" s="27">
-        <f t="shared" si="1"/>
+        <f>(E22-D22)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4758,7 +4835,7 @@
       <c r="F23" s="34"/>
       <c r="G23" s="17"/>
       <c r="H23" s="27">
-        <f t="shared" si="1"/>
+        <f>(E23-D23)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4771,7 +4848,7 @@
       <c r="F24" s="34"/>
       <c r="G24" s="17"/>
       <c r="H24" s="27">
-        <f t="shared" si="1"/>
+        <f>(E24-D24)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4784,7 +4861,7 @@
       <c r="F25" s="34"/>
       <c r="G25" s="17"/>
       <c r="H25" s="27">
-        <f t="shared" si="1"/>
+        <f>(E25-D25)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4797,7 +4874,7 @@
       <c r="F26" s="34"/>
       <c r="G26" s="17"/>
       <c r="H26" s="27">
-        <f t="shared" si="1"/>
+        <f>(E26-D26)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4810,7 +4887,7 @@
       <c r="F27" s="34"/>
       <c r="G27" s="17"/>
       <c r="H27" s="27">
-        <f t="shared" si="1"/>
+        <f>(E27-D27)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4823,7 +4900,7 @@
       <c r="F28" s="34"/>
       <c r="G28" s="17"/>
       <c r="H28" s="27">
-        <f t="shared" si="1"/>
+        <f>(E28-D28)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4836,7 +4913,7 @@
       <c r="F29" s="34"/>
       <c r="G29" s="17"/>
       <c r="H29" s="27">
-        <f t="shared" si="1"/>
+        <f>(E29-D29)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4849,7 +4926,7 @@
       <c r="F30" s="34"/>
       <c r="G30" s="17"/>
       <c r="H30" s="27">
-        <f t="shared" si="1"/>
+        <f>(E30-D30)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4862,7 +4939,7 @@
       <c r="F31" s="34"/>
       <c r="G31" s="17"/>
       <c r="H31" s="27">
-        <f t="shared" si="1"/>
+        <f>(E31-D31)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4875,7 +4952,7 @@
       <c r="F32" s="34"/>
       <c r="G32" s="17"/>
       <c r="H32" s="27">
-        <f t="shared" si="1"/>
+        <f>(E32-D32)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4888,7 +4965,7 @@
       <c r="F33" s="34"/>
       <c r="G33" s="17"/>
       <c r="H33" s="27">
-        <f t="shared" si="1"/>
+        <f>(E33-D33)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4901,7 +4978,7 @@
       <c r="F34" s="34"/>
       <c r="G34" s="17"/>
       <c r="H34" s="27">
-        <f t="shared" si="1"/>
+        <f>(E34-D34)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4914,7 +4991,7 @@
       <c r="F35" s="34"/>
       <c r="G35" s="17"/>
       <c r="H35" s="27">
-        <f t="shared" si="1"/>
+        <f>(E35-D35)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4927,7 +5004,7 @@
       <c r="F36" s="34"/>
       <c r="G36" s="17"/>
       <c r="H36" s="27">
-        <f t="shared" si="1"/>
+        <f>(E36-D36)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4940,7 +5017,7 @@
       <c r="F37" s="34"/>
       <c r="G37" s="17"/>
       <c r="H37" s="27">
-        <f t="shared" si="1"/>
+        <f>(E37-D37)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4953,7 +5030,7 @@
       <c r="F38" s="34"/>
       <c r="G38" s="17"/>
       <c r="H38" s="27">
-        <f t="shared" si="1"/>
+        <f>(E38-D38)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4966,7 +5043,7 @@
       <c r="F39" s="34"/>
       <c r="G39" s="17"/>
       <c r="H39" s="27">
-        <f t="shared" si="1"/>
+        <f>(E39-D39)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4979,7 +5056,7 @@
       <c r="F40" s="34"/>
       <c r="G40" s="17"/>
       <c r="H40" s="27">
-        <f t="shared" si="1"/>
+        <f>(E40-D40)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -4992,7 +5069,7 @@
       <c r="F41" s="34"/>
       <c r="G41" s="17"/>
       <c r="H41" s="27">
-        <f t="shared" si="1"/>
+        <f>(E41-D41)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5005,7 +5082,7 @@
       <c r="F42" s="34"/>
       <c r="G42" s="17"/>
       <c r="H42" s="27">
-        <f t="shared" si="1"/>
+        <f>(E42-D42)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5018,7 +5095,7 @@
       <c r="F43" s="34"/>
       <c r="G43" s="17"/>
       <c r="H43" s="27">
-        <f t="shared" si="1"/>
+        <f>(E43-D43)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5031,7 +5108,7 @@
       <c r="F44" s="34"/>
       <c r="G44" s="17"/>
       <c r="H44" s="27">
-        <f t="shared" si="1"/>
+        <f>(E44-D44)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5044,7 +5121,7 @@
       <c r="F45" s="34"/>
       <c r="G45" s="17"/>
       <c r="H45" s="27">
-        <f t="shared" si="1"/>
+        <f>(E45-D45)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5057,7 +5134,7 @@
       <c r="F46" s="34"/>
       <c r="G46" s="17"/>
       <c r="H46" s="27">
-        <f t="shared" si="1"/>
+        <f>(E46-D46)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5070,7 +5147,7 @@
       <c r="F47" s="34"/>
       <c r="G47" s="17"/>
       <c r="H47" s="27">
-        <f t="shared" si="1"/>
+        <f>(E47-D47)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5083,7 +5160,7 @@
       <c r="F48" s="34"/>
       <c r="G48" s="17"/>
       <c r="H48" s="27">
-        <f t="shared" si="1"/>
+        <f>(E48-D48)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5096,7 +5173,7 @@
       <c r="F49" s="34"/>
       <c r="G49" s="17"/>
       <c r="H49" s="27">
-        <f t="shared" si="1"/>
+        <f>(E49-D49)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5109,7 +5186,7 @@
       <c r="F50" s="34"/>
       <c r="G50" s="17"/>
       <c r="H50" s="27">
-        <f t="shared" si="1"/>
+        <f>(E50-D50)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5122,7 +5199,7 @@
       <c r="F51" s="34"/>
       <c r="G51" s="17"/>
       <c r="H51" s="27">
-        <f t="shared" si="1"/>
+        <f>(E51-D51)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5135,7 +5212,7 @@
       <c r="F52" s="34"/>
       <c r="G52" s="17"/>
       <c r="H52" s="27">
-        <f t="shared" si="1"/>
+        <f>(E52-D52)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5148,7 +5225,7 @@
       <c r="F53" s="34"/>
       <c r="G53" s="17"/>
       <c r="H53" s="27">
-        <f t="shared" si="1"/>
+        <f>(E53-D53)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5161,7 +5238,7 @@
       <c r="F54" s="34"/>
       <c r="G54" s="17"/>
       <c r="H54" s="27">
-        <f t="shared" si="1"/>
+        <f>(E54-D54)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5174,7 +5251,7 @@
       <c r="F55" s="34"/>
       <c r="G55" s="17"/>
       <c r="H55" s="27">
-        <f t="shared" si="1"/>
+        <f>(E55-D55)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5187,7 +5264,7 @@
       <c r="F56" s="34"/>
       <c r="G56" s="17"/>
       <c r="H56" s="27">
-        <f t="shared" si="1"/>
+        <f>(E56-D56)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5200,7 +5277,7 @@
       <c r="F57" s="34"/>
       <c r="G57" s="17"/>
       <c r="H57" s="27">
-        <f t="shared" si="1"/>
+        <f>(E57-D57)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5213,7 +5290,7 @@
       <c r="F58" s="34"/>
       <c r="G58" s="17"/>
       <c r="H58" s="27">
-        <f t="shared" si="1"/>
+        <f>(E58-D58)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5226,7 +5303,7 @@
       <c r="F59" s="34"/>
       <c r="G59" s="17"/>
       <c r="H59" s="27">
-        <f t="shared" si="1"/>
+        <f>(E59-D59)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5239,7 +5316,7 @@
       <c r="F60" s="34"/>
       <c r="G60" s="17"/>
       <c r="H60" s="27">
-        <f t="shared" si="1"/>
+        <f>(E60-D60)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5252,7 +5329,7 @@
       <c r="F61" s="34"/>
       <c r="G61" s="17"/>
       <c r="H61" s="27">
-        <f t="shared" si="1"/>
+        <f>(E61-D61)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5265,7 +5342,7 @@
       <c r="F62" s="34"/>
       <c r="G62" s="17"/>
       <c r="H62" s="27">
-        <f t="shared" si="1"/>
+        <f>(E62-D62)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5278,7 +5355,7 @@
       <c r="F63" s="34"/>
       <c r="G63" s="17"/>
       <c r="H63" s="27">
-        <f t="shared" si="1"/>
+        <f>(E63-D63)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5291,7 +5368,7 @@
       <c r="F64" s="34"/>
       <c r="G64" s="17"/>
       <c r="H64" s="27">
-        <f t="shared" si="1"/>
+        <f>(E64-D64)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5304,7 +5381,7 @@
       <c r="F65" s="34"/>
       <c r="G65" s="17"/>
       <c r="H65" s="27">
-        <f t="shared" si="1"/>
+        <f>(E65-D65)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5317,7 +5394,7 @@
       <c r="F66" s="34"/>
       <c r="G66" s="17"/>
       <c r="H66" s="27">
-        <f t="shared" si="1"/>
+        <f>(E66-D66)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5330,7 +5407,7 @@
       <c r="F67" s="34"/>
       <c r="G67" s="17"/>
       <c r="H67" s="27">
-        <f t="shared" si="1"/>
+        <f>(E67-D67)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5343,7 +5420,7 @@
       <c r="F68" s="34"/>
       <c r="G68" s="17"/>
       <c r="H68" s="27">
-        <f t="shared" si="1"/>
+        <f>(E68-D68)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5356,7 +5433,7 @@
       <c r="F69" s="34"/>
       <c r="G69" s="17"/>
       <c r="H69" s="27">
-        <f t="shared" si="1"/>
+        <f>(E69-D69)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5369,7 +5446,7 @@
       <c r="F70" s="34"/>
       <c r="G70" s="17"/>
       <c r="H70" s="27">
-        <f t="shared" si="1"/>
+        <f>(E70-D70)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5382,7 +5459,7 @@
       <c r="F71" s="34"/>
       <c r="G71" s="17"/>
       <c r="H71" s="27">
-        <f t="shared" si="1"/>
+        <f>(E71-D71)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5395,7 +5472,7 @@
       <c r="F72" s="34"/>
       <c r="G72" s="17"/>
       <c r="H72" s="27">
-        <f t="shared" ref="H72:H78" si="2">(E72-D72)*24</f>
+        <f t="shared" ref="H72:H78" si="0">(E72-D72)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5408,7 +5485,7 @@
       <c r="F73" s="34"/>
       <c r="G73" s="17"/>
       <c r="H73" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -5421,7 +5498,7 @@
       <c r="F74" s="34"/>
       <c r="G74" s="17"/>
       <c r="H74" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -5434,7 +5511,7 @@
       <c r="F75" s="34"/>
       <c r="G75" s="17"/>
       <c r="H75" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -5447,7 +5524,7 @@
       <c r="F76" s="34"/>
       <c r="G76" s="17"/>
       <c r="H76" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -5460,7 +5537,7 @@
       <c r="F77" s="34"/>
       <c r="G77" s="17"/>
       <c r="H77" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -5473,7 +5550,7 @@
       <c r="F78" s="36"/>
       <c r="G78" s="18"/>
       <c r="H78" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -5481,7 +5558,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>0</v>
+        <v>7.6333333333333346</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ShiftUnit FunctionalSim all test cases passed
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-0799-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-0799-350-1201.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5262716E-38E9-4B36-A889-4EF20F2B97C7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDDC44CC-5AAC-4177-A038-01B90B1AFE01}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2400" windowHeight="585" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log - Part 1" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Activity Log - Part 3" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -155,7 +154,13 @@
     <t>Finished implementation of SRA</t>
   </si>
   <si>
-    <t>Reviewed group's code</t>
+    <t>Reviewed group's code; fixed compilation errors</t>
+  </si>
+  <si>
+    <t>Fixed logic errors for ShiftUnit</t>
+  </si>
+  <si>
+    <t>Fixed logic errors for SRA, SLL and SRL</t>
   </si>
 </sst>
 </file>
@@ -2717,8 +2722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD091BD6-3364-44DE-8BB4-985458F62AD8}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2897,7 +2902,7 @@
         <v>779</v>
       </c>
       <c r="C10" s="22">
-        <v>43931</v>
+        <v>43932</v>
       </c>
       <c r="D10" s="20">
         <v>0.58958333333333335</v>
@@ -2920,7 +2925,7 @@
         <v>779</v>
       </c>
       <c r="C11" s="22">
-        <v>43931</v>
+        <v>43932</v>
       </c>
       <c r="D11" s="20">
         <v>0.83611111111111114</v>
@@ -2943,7 +2948,7 @@
         <v>779</v>
       </c>
       <c r="C12" s="22">
-        <v>43932</v>
+        <v>43933</v>
       </c>
       <c r="D12" s="20">
         <v>0.4381944444444445</v>
@@ -2966,7 +2971,7 @@
         <v>779</v>
       </c>
       <c r="C13" s="22">
-        <v>43932</v>
+        <v>43933</v>
       </c>
       <c r="D13" s="20">
         <v>0.62916666666666665</v>
@@ -2987,7 +2992,7 @@
       <c r="A14" s="33"/>
       <c r="B14" s="14"/>
       <c r="C14" s="22">
-        <v>43932</v>
+        <v>43933</v>
       </c>
       <c r="D14" s="20">
         <v>0.67152777777777783</v>
@@ -3007,7 +3012,9 @@
     <row r="15" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="33"/>
       <c r="B15" s="14"/>
-      <c r="C15" s="22"/>
+      <c r="C15" s="22">
+        <v>43933</v>
+      </c>
       <c r="D15" s="20">
         <v>0.74375000000000002</v>
       </c>
@@ -3026,40 +3033,56 @@
     <row r="16" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33"/>
       <c r="B16" s="14"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="23"/>
+      <c r="C16" s="22">
+        <v>43934</v>
+      </c>
+      <c r="D16" s="20">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E16" s="23">
+        <v>0.41944444444444445</v>
+      </c>
       <c r="F16" s="34"/>
-      <c r="G16" s="17"/>
+      <c r="G16" s="17" t="s">
+        <v>26</v>
+      </c>
       <c r="H16" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5666666666666664</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33"/>
       <c r="B17" s="14"/>
       <c r="C17" s="22"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="23"/>
+      <c r="D17" s="20">
+        <v>0.58263888888888882</v>
+      </c>
+      <c r="E17" s="23">
+        <v>0.73125000000000007</v>
+      </c>
       <c r="F17" s="34"/>
-      <c r="G17" s="17"/>
+      <c r="G17" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="H17" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.56666666666667</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33"/>
       <c r="B18" s="14"/>
       <c r="C18" s="22"/>
-      <c r="D18" s="20"/>
+      <c r="D18" s="20">
+        <v>0.73125000000000007</v>
+      </c>
       <c r="E18" s="23"/>
       <c r="F18" s="34"/>
       <c r="G18" s="17"/>
       <c r="H18" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-17.55</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3846,7 +3869,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>9.0999999999999961</v>
+        <v>-3.3166666666666682</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed ExecUnit (passes all functinalsim cases)
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-0799-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-0799-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E203893-4955-4490-B585-62A3C10CAE0D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11136696-26B1-4146-A8B1-1473C612A270}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t>Fixed logic errors for SRA, SLL and SRL</t>
+  </si>
+  <si>
+    <t>Fixed some errors that showed up in our modified ArithUnit.vhd</t>
+  </si>
+  <si>
+    <t>Fixed logic errors for ExecUnit.vhd</t>
+  </si>
+  <si>
+    <t>Fixed logic errors in ExecUnit and ShiftUnit, now passes all test cases</t>
   </si>
 </sst>
 </file>
@@ -2722,8 +2731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD091BD6-3364-44DE-8BB4-985458F62AD8}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3093,39 +3102,57 @@
       <c r="A19" s="33"/>
       <c r="B19" s="14"/>
       <c r="C19" s="22"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="23"/>
+      <c r="D19" s="20">
+        <v>0.34375</v>
+      </c>
+      <c r="E19" s="23">
+        <v>0.3527777777777778</v>
+      </c>
       <c r="F19" s="34"/>
-      <c r="G19" s="17"/>
+      <c r="G19" s="17" t="s">
+        <v>27</v>
+      </c>
       <c r="H19" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.21666666666666723</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="33"/>
       <c r="B20" s="14"/>
       <c r="C20" s="22"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="23"/>
+      <c r="D20" s="20">
+        <v>0.3527777777777778</v>
+      </c>
+      <c r="E20" s="23">
+        <v>0.3666666666666667</v>
+      </c>
       <c r="F20" s="34"/>
-      <c r="G20" s="17"/>
+      <c r="G20" s="17" t="s">
+        <v>28</v>
+      </c>
       <c r="H20" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333348</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="33"/>
       <c r="B21" s="14"/>
       <c r="C21" s="22"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="23"/>
+      <c r="D21" s="20">
+        <v>0.6645833333333333</v>
+      </c>
+      <c r="E21" s="23">
+        <v>0.71388888888888891</v>
+      </c>
       <c r="F21" s="34"/>
-      <c r="G21" s="17"/>
+      <c r="G21" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="H21" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.1833333333333345</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3873,7 +3900,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>15.68333333333333</v>
+        <v>17.416666666666664</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TODOs done, added netlist RTL screenshots
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-0799-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-0799-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11136696-26B1-4146-A8B1-1473C612A270}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78392E27-B102-4F96-AB34-8A7A5B33CF74}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -121,31 +121,10 @@
     <t>Duration</t>
   </si>
   <si>
-    <t>Gxx</t>
-  </si>
-  <si>
     <t>Ruelt Yean (Ryan), Kiew</t>
   </si>
   <si>
     <t>G47</t>
-  </si>
-  <si>
-    <t>Read through Part 2 pdf</t>
-  </si>
-  <si>
-    <t>Reviewed Barrel Shifter design implementation</t>
-  </si>
-  <si>
-    <t>First implementation  of Barrel Shifter</t>
-  </si>
-  <si>
-    <t>Second implementation of Barrel Shifter; attempting to use same MUX entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Third implementaiton of Barrel Shifter; error fixing, split MUX into three entities </t>
-  </si>
-  <si>
-    <t>Fixing compilation errors for second implementation</t>
   </si>
   <si>
     <t>Finished implementation of SLL and SRL</t>
@@ -163,13 +142,55 @@
     <t>Fixed logic errors for SRA, SLL and SRL</t>
   </si>
   <si>
-    <t>Fixed some errors that showed up in our modified ArithUnit.vhd</t>
+    <t>Fixed logic errors in ExecUnit and ShiftUnit, now passes all test cases (DONE)</t>
   </si>
   <si>
-    <t>Fixed logic errors for ExecUnit.vhd</t>
+    <t>Read through Part 2 pdf and set up project folder for initial compilation</t>
   </si>
   <si>
-    <t>Fixed logic errors in ExecUnit and ShiftUnit, now passes all test cases</t>
+    <t>Reviewed Barrel Shifter design implementation - reviewed notes and online sources</t>
+  </si>
+  <si>
+    <t>First implementation  of Barrel Shifter - uses 3 different MUX's for simplicity</t>
+  </si>
+  <si>
+    <t>Second implementation of Barrel Shifter - attempting to use one MUX entity</t>
+  </si>
+  <si>
+    <t>Fixing compilation errors for second implementation of Barrel Shifters</t>
+  </si>
+  <si>
+    <t>Fixing compilation errors for second implementation of Barrel Shifters (DONE)</t>
+  </si>
+  <si>
+    <t>Third implementaiton of Barrel Shifter - instead of using complicated logic within MUX, just pass options into MUX</t>
+  </si>
+  <si>
+    <t>Fixed some errors that showed up in our modified ArithUnit.vhd - wrong parameters were being passed</t>
+  </si>
+  <si>
+    <t>Fixed logic errors for ShiftUnit (DONE) - implemented 32-bit shifting for a shift of more than 32 bits</t>
+  </si>
+  <si>
+    <t>Fixed logic errors for ExecUnit</t>
+  </si>
+  <si>
+    <t>Compiling functional simulation screenshots for ShiftUnit</t>
+  </si>
+  <si>
+    <t>Compiling timing simulation screenshots for ShiftUnit</t>
+  </si>
+  <si>
+    <t>Compiling timing simulation screenshots for ShiftUnit (DONE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compiling functional and timing simulation screenshots for ExecUnit </t>
+  </si>
+  <si>
+    <t>Adding comments to code for clarification</t>
+  </si>
+  <si>
+    <t>Compiling RTL netlost viewer screenshots for ShiftUnit and ExecUnit</t>
   </si>
 </sst>
 </file>
@@ -969,7 +990,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,7 +1010,9 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="37" t="s">
+        <v>13</v>
+      </c>
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
       <c r="E1" s="38" t="s">
@@ -1002,7 +1025,9 @@
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="39"/>
+      <c r="B2" s="39">
+        <v>301290779</v>
+      </c>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
       <c r="E2" s="38"/>
@@ -1014,7 +1039,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
@@ -2731,8 +2756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD091BD6-3364-44DE-8BB4-985458F62AD8}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2752,7 +2777,9 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="37" t="s">
+        <v>13</v>
+      </c>
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
       <c r="E1" s="38" t="s">
@@ -2765,7 +2792,9 @@
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="39"/>
+      <c r="B2" s="39">
+        <v>301290779</v>
+      </c>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
       <c r="E2" s="38"/>
@@ -2777,7 +2806,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
@@ -2828,7 +2857,7 @@
       </c>
       <c r="F6" s="32"/>
       <c r="G6" s="16" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H6" s="12">
         <f t="shared" ref="H6:H11" si="0">(E6-D6)*24</f>
@@ -2852,7 +2881,7 @@
       </c>
       <c r="F7" s="34"/>
       <c r="G7" s="17" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H7" s="27">
         <f t="shared" si="0"/>
@@ -2875,7 +2904,7 @@
       </c>
       <c r="F8" s="34"/>
       <c r="G8" s="17" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H8" s="27">
         <f t="shared" si="0"/>
@@ -2898,7 +2927,7 @@
       </c>
       <c r="F9" s="34"/>
       <c r="G9" s="17" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H9" s="27">
         <f t="shared" si="0"/>
@@ -2921,7 +2950,7 @@
       </c>
       <c r="F10" s="34"/>
       <c r="G10" s="17" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H10" s="27">
         <f t="shared" si="0"/>
@@ -2944,7 +2973,7 @@
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="17" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="H11" s="27">
         <f t="shared" si="0"/>
@@ -2967,7 +2996,7 @@
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="17" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H12" s="27">
         <f t="shared" ref="H12:H71" si="1">(E12-D12)*24</f>
@@ -2990,7 +3019,7 @@
       </c>
       <c r="F13" s="34"/>
       <c r="G13" s="17" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H13" s="27">
         <f t="shared" si="1"/>
@@ -2999,7 +3028,9 @@
     </row>
     <row r="14" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="33"/>
-      <c r="B14" s="14"/>
+      <c r="B14" s="14">
+        <v>779</v>
+      </c>
       <c r="C14" s="22">
         <v>43933</v>
       </c>
@@ -3011,7 +3042,7 @@
       </c>
       <c r="F14" s="34"/>
       <c r="G14" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="H14" s="27">
         <f t="shared" si="1"/>
@@ -3020,7 +3051,9 @@
     </row>
     <row r="15" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="33"/>
-      <c r="B15" s="14"/>
+      <c r="B15" s="14">
+        <v>779</v>
+      </c>
       <c r="C15" s="22">
         <v>43933</v>
       </c>
@@ -3032,7 +3065,7 @@
       </c>
       <c r="F15" s="34"/>
       <c r="G15" s="17" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="H15" s="27">
         <f t="shared" si="1"/>
@@ -3041,7 +3074,9 @@
     </row>
     <row r="16" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33"/>
-      <c r="B16" s="14"/>
+      <c r="B16" s="14">
+        <v>779</v>
+      </c>
       <c r="C16" s="22">
         <v>43934</v>
       </c>
@@ -3053,7 +3088,7 @@
       </c>
       <c r="F16" s="34"/>
       <c r="G16" s="17" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H16" s="27">
         <f t="shared" si="1"/>
@@ -3062,8 +3097,12 @@
     </row>
     <row r="17" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="22"/>
+      <c r="B17" s="14">
+        <v>779</v>
+      </c>
+      <c r="C17" s="22">
+        <v>43934</v>
+      </c>
       <c r="D17" s="20">
         <v>0.58263888888888882</v>
       </c>
@@ -3072,7 +3111,7 @@
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="17" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H17" s="27">
         <f t="shared" si="1"/>
@@ -3081,8 +3120,12 @@
     </row>
     <row r="18" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="22"/>
+      <c r="B18" s="14">
+        <v>779</v>
+      </c>
+      <c r="C18" s="22">
+        <v>43934</v>
+      </c>
       <c r="D18" s="20">
         <v>0.73125000000000007</v>
       </c>
@@ -3091,7 +3134,7 @@
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="17" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H18" s="27">
         <f t="shared" si="1"/>
@@ -3100,8 +3143,12 @@
     </row>
     <row r="19" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="33"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="22"/>
+      <c r="B19" s="14">
+        <v>779</v>
+      </c>
+      <c r="C19" s="22">
+        <v>43935</v>
+      </c>
       <c r="D19" s="20">
         <v>0.34375</v>
       </c>
@@ -3110,7 +3157,7 @@
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H19" s="27">
         <f t="shared" si="1"/>
@@ -3119,8 +3166,12 @@
     </row>
     <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="33"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="22"/>
+      <c r="B20" s="14">
+        <v>779</v>
+      </c>
+      <c r="C20" s="22">
+        <v>43935</v>
+      </c>
       <c r="D20" s="20">
         <v>0.3527777777777778</v>
       </c>
@@ -3129,7 +3180,7 @@
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H20" s="27">
         <f t="shared" si="1"/>
@@ -3138,8 +3189,12 @@
     </row>
     <row r="21" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="33"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="22"/>
+      <c r="B21" s="14">
+        <v>779</v>
+      </c>
+      <c r="C21" s="22">
+        <v>43935</v>
+      </c>
       <c r="D21" s="20">
         <v>0.6645833333333333</v>
       </c>
@@ -3148,7 +3203,7 @@
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="17" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H21" s="27">
         <f t="shared" si="1"/>
@@ -3157,80 +3212,140 @@
     </row>
     <row r="22" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="33"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="23"/>
+      <c r="B22" s="14">
+        <v>779</v>
+      </c>
+      <c r="C22" s="22">
+        <v>43936</v>
+      </c>
+      <c r="D22" s="20">
+        <v>0.84375</v>
+      </c>
+      <c r="E22" s="23">
+        <v>0.88124999999999998</v>
+      </c>
       <c r="F22" s="34"/>
-      <c r="G22" s="17"/>
+      <c r="G22" s="17" t="s">
+        <v>31</v>
+      </c>
       <c r="H22" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.89999999999999947</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="33"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="23"/>
+      <c r="B23" s="14">
+        <v>779</v>
+      </c>
+      <c r="C23" s="22">
+        <v>43936</v>
+      </c>
+      <c r="D23" s="20">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="E23" s="23">
+        <v>0.93055555555555547</v>
+      </c>
       <c r="F23" s="34"/>
-      <c r="G23" s="17"/>
+      <c r="G23" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="H23" s="27">
         <f>(E23-D23)*24</f>
-        <v>0</v>
+        <v>0.83333333333333037</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="33"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="23"/>
+      <c r="B24" s="14">
+        <v>779</v>
+      </c>
+      <c r="C24" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D24" s="20">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="E24" s="23">
+        <v>0.39374999999999999</v>
+      </c>
       <c r="F24" s="34"/>
-      <c r="G24" s="17"/>
+      <c r="G24" s="17" t="s">
+        <v>33</v>
+      </c>
       <c r="H24" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.0666666666666669</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="33"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="23"/>
+      <c r="B25" s="14">
+        <v>779</v>
+      </c>
+      <c r="C25" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D25" s="20">
+        <v>0.39374999999999999</v>
+      </c>
+      <c r="E25" s="23">
+        <v>0.4055555555555555</v>
+      </c>
       <c r="F25" s="34"/>
-      <c r="G25" s="17"/>
+      <c r="G25" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="H25" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.28333333333333233</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="33"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="23"/>
+      <c r="B26" s="14">
+        <v>779</v>
+      </c>
+      <c r="C26" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D26" s="20">
+        <v>0.5854166666666667</v>
+      </c>
+      <c r="E26" s="23">
+        <v>0.59861111111111109</v>
+      </c>
       <c r="F26" s="34"/>
-      <c r="G26" s="17"/>
+      <c r="G26" s="17" t="s">
+        <v>35</v>
+      </c>
       <c r="H26" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.31666666666666554</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="33"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="23"/>
+      <c r="B27" s="14">
+        <v>779</v>
+      </c>
+      <c r="C27" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D27" s="20">
+        <v>0.59861111111111109</v>
+      </c>
+      <c r="E27" s="23">
+        <v>0.61527777777777781</v>
+      </c>
       <c r="F27" s="34"/>
-      <c r="G27" s="17"/>
+      <c r="G27" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="H27" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.40000000000000124</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3900,7 +4015,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>17.416666666666664</v>
+        <v>21.216666666666658</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4650,7 +4765,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
@@ -4678,7 +4793,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>

</xml_diff>

<commit_message>
Added some circuit diagrams
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-0799-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-0799-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78392E27-B102-4F96-AB34-8A7A5B33CF74}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D59ACBD-6646-44D1-BF22-953AE1D4BBF9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -190,7 +190,10 @@
     <t>Adding comments to code for clarification</t>
   </si>
   <si>
-    <t>Compiling RTL netlost viewer screenshots for ShiftUnit and ExecUnit</t>
+    <t>Compiling RTL netlist viewer screenshots for ShiftUnit and ExecUnit</t>
+  </si>
+  <si>
+    <t>Writing ShiftUnit section for report</t>
   </si>
 </sst>
 </file>
@@ -2756,8 +2759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD091BD6-3364-44DE-8BB4-985458F62AD8}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3350,15 +3353,25 @@
     </row>
     <row r="28" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="33"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="23"/>
+      <c r="B28" s="14">
+        <v>779</v>
+      </c>
+      <c r="C28" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D28" s="20">
+        <v>0.84930555555555554</v>
+      </c>
+      <c r="E28" s="23">
+        <v>0.94791666666666663</v>
+      </c>
       <c r="F28" s="34"/>
-      <c r="G28" s="17"/>
+      <c r="G28" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="H28" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.3666666666666663</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4015,7 +4028,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>21.216666666666658</v>
+        <v>23.583333333333325</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
annotated waveforms and rtl circuits
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-0799-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-0799-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C45C209-3A94-47EC-A073-F0A617E5956D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A017F13-E5D7-4EF2-BCE5-F68EE2B70CB6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Annotating waveforms and writing ShiftUnit functional simulation section of report</t>
+  </si>
+  <si>
+    <t>Annotating waveforms and writing ShiftUnit timing simulation section of report</t>
   </si>
 </sst>
 </file>
@@ -2763,7 +2766,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3402,13 +3405,19 @@
       <c r="A30" s="33"/>
       <c r="B30" s="14"/>
       <c r="C30" s="22"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="23"/>
+      <c r="D30" s="20">
+        <v>0.42638888888888887</v>
+      </c>
+      <c r="E30" s="23">
+        <v>0.5229166666666667</v>
+      </c>
       <c r="F30" s="34"/>
-      <c r="G30" s="17"/>
+      <c r="G30" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="H30" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.3166666666666678</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4039,7 +4048,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>25.633333333333326</v>
+        <v>27.949999999999992</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
annotated some FXU waveforms
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-0799-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-0799-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A017F13-E5D7-4EF2-BCE5-F68EE2B70CB6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD05064-37EE-4714-A97A-573CB66F5FB7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -200,6 +200,15 @@
   </si>
   <si>
     <t>Annotating waveforms and writing ShiftUnit timing simulation section of report</t>
+  </si>
+  <si>
+    <t>Annotating waveforms and writing ShiftUnit timing simulation section of report (DONE)</t>
+  </si>
+  <si>
+    <t>Annotating netlist RTL circuit of ShiftUnit and writing ShiftUnit synthesis section of report</t>
+  </si>
+  <si>
+    <t>Annotating ExecUnit waveforms</t>
   </si>
 </sst>
 </file>
@@ -2765,8 +2774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD091BD6-3364-44DE-8BB4-985458F62AD8}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3404,7 +3413,9 @@
     <row r="30" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="33"/>
       <c r="B30" s="14"/>
-      <c r="C30" s="22"/>
+      <c r="C30" s="22">
+        <v>43938</v>
+      </c>
       <c r="D30" s="20">
         <v>0.42638888888888887</v>
       </c>
@@ -3423,40 +3434,62 @@
     <row r="31" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="33"/>
       <c r="B31" s="14"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="23"/>
+      <c r="C31" s="22">
+        <v>43938</v>
+      </c>
+      <c r="D31" s="20">
+        <v>0.64027777777777783</v>
+      </c>
+      <c r="E31" s="23">
+        <v>0.77222222222222225</v>
+      </c>
       <c r="F31" s="34"/>
-      <c r="G31" s="17"/>
+      <c r="G31" s="17" t="s">
+        <v>40</v>
+      </c>
       <c r="H31" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.1666666666666661</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="33"/>
       <c r="B32" s="14"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="23"/>
+      <c r="C32" s="22">
+        <v>43938</v>
+      </c>
+      <c r="D32" s="20">
+        <v>0.77222222222222225</v>
+      </c>
+      <c r="E32" s="23">
+        <v>0.83194444444444438</v>
+      </c>
       <c r="F32" s="34"/>
-      <c r="G32" s="17"/>
+      <c r="G32" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="H32" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.4333333333333309</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="33"/>
       <c r="B33" s="14"/>
       <c r="C33" s="22"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="23"/>
+      <c r="D33" s="20">
+        <v>0.87708333333333333</v>
+      </c>
+      <c r="E33" s="23">
+        <v>0.89166666666666661</v>
+      </c>
       <c r="F33" s="34"/>
-      <c r="G33" s="17"/>
+      <c r="G33" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="H33" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.34999999999999876</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4048,7 +4081,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>27.949999999999992</v>
+        <v>32.899999999999991</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>